<commit_message>
Working on clearance correction
</commit_message>
<xml_diff>
--- a/experimental_data/GEC/Waldstein1960.xlsx
+++ b/experimental_data/GEC/Waldstein1960.xlsx
@@ -420,7 +420,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -637,11 +637,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="91895687"/>
-        <c:axId val="62369559"/>
+        <c:axId val="49807467"/>
+        <c:axId val="54423879"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91895687"/>
+        <c:axId val="49807467"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -677,11 +677,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="62369559"/>
+        <c:crossAx val="54423879"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="62369559"/>
+        <c:axId val="54423879"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -717,7 +717,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="91895687"/>
+        <c:crossAx val="49807467"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -742,7 +742,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -928,11 +928,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="63914409"/>
-        <c:axId val="64171944"/>
+        <c:axId val="45995052"/>
+        <c:axId val="70454418"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63914409"/>
+        <c:axId val="45995052"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -968,11 +968,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="64171944"/>
+        <c:crossAx val="70454418"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64171944"/>
+        <c:axId val="70454418"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1008,7 +1008,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="63914409"/>
+        <c:crossAx val="45995052"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1033,7 +1033,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1241,11 +1241,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="41388585"/>
-        <c:axId val="27036683"/>
+        <c:axId val="82948773"/>
+        <c:axId val="43927778"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="41388585"/>
+        <c:axId val="82948773"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1281,11 +1281,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="27036683"/>
+        <c:crossAx val="43927778"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="27036683"/>
+        <c:axId val="43927778"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1321,7 +1321,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="41388585"/>
+        <c:crossAx val="82948773"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1437,7 +1437,7 @@
       <xdr:col>24</xdr:col>
       <xdr:colOff>702720</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>41040</xdr:rowOff>
+      <xdr:rowOff>46800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1536,7 +1536,7 @@
       <xdr:col>21</xdr:col>
       <xdr:colOff>399240</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>123120</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1565,8 +1565,8 @@
   </sheetPr>
   <dimension ref="A1:V61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M40" activeCellId="0" sqref="M40"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O12" activeCellId="0" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3152,7 +3152,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="7" t="s">
         <v>11</v>
       </c>

</xml_diff>